<commit_message>
add the data to df_com
</commit_message>
<xml_diff>
--- a/community.xlsx
+++ b/community.xlsx
@@ -240,10 +240,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -296,6 +296,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -311,7 +334,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -319,24 +342,25 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -356,31 +380,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -394,47 +411,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -449,19 +449,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,91 +605,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,67 +623,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,6 +640,51 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -676,51 +721,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -745,7 +745,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -763,134 +763,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -900,11 +900,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -912,11 +909,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1246,7 +1243,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8421052631579" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1257,7 +1254,7 @@
     <col min="4" max="4" width="28.8947368421053" customWidth="1"/>
     <col min="5" max="5" width="6.73684210526316" customWidth="1"/>
     <col min="6" max="6" width="16.3157894736842" customWidth="1"/>
-    <col min="7" max="7" width="34.1578947368421" customWidth="1"/>
+    <col min="7" max="7" width="45.2631578947368" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1270,498 +1267,498 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>8500</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>1154</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>283</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>7850</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>801</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>945</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>6900</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>432</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>980</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>10832</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>1303</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>256</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>9000</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>704</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>479</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>6500</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>887</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>286</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>13620</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>163</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>569</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>24120</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>577</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>718</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="1">
         <v>24000</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>1065</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>816</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>13563</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>381</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>826</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>10754</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>466</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>467</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>11178</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>312</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>332</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>12546</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>1742</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>578</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>8321</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>1118</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>668</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>1262</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <v>864</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>647</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <v>625</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>1419</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <v>812</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="7" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>6218</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>935</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>510</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="7" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>11700</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>1122</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>484</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="7" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>12069</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>1439</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>780</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="7" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="8">
         <v>10790</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>751</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>271</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="7" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="23" spans="4:4">
-      <c r="D23" s="10"/>
+      <c r="D23" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
draw the heat map
</commit_message>
<xml_diff>
--- a/community.xlsx
+++ b/community.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,40 +436,45 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>社区名称</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>地址</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>常住人口</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>发热诊室</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>标记名称</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>w</t>
         </is>
@@ -479,771 +484,834 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>金山街道金洲社区</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>福州市仓山区金环路5号</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>8500</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>金洲社区卫生服务站</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>1154</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>283</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>福建省福州市仓山区金环路5号</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>0.03637943771592936</v>
+      <c r="J2" t="n">
+        <v>0.6605496581398433</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>金山街道幸福社区</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>仓山区浦上大道418号泰禾红峪A14号楼一层</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>7850</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>丽景社区卫生服务站</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>801</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>945</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>福建省福州市仓山区葛屿路</t>
         </is>
       </c>
-      <c r="I3" t="n">
-        <v>0.05228704727139491</v>
+      <c r="J3" t="n">
+        <v>0.949387713739693</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>金山街道六江道社区</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>福州市仓山区金桔路826号68栋旁</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>6900</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>中天社区卫生服务站</t>
         </is>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>432</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>980</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>福建省福州市仓山区金桔路</t>
         </is>
       </c>
-      <c r="I4" t="n">
-        <v>0.04580161226689081</v>
+      <c r="J4" t="n">
+        <v>0.8316302071898446</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>金山街道金环社区</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>福州市仓山区金山街道金榕南路10号榕城广场8号楼一层</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>10832</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>金洲社区卫生服务站</t>
         </is>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>1303</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>256</v>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>福建省福州市仓山区友兰路</t>
         </is>
       </c>
-      <c r="I5" t="n">
-        <v>0.03637943771592936</v>
+      <c r="J5" t="n">
+        <v>0.6605496581398433</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>金山街道鑫龙社区</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>福州市仓山区石边支路1号</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>9000</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>丽景社区卫生服务站</t>
         </is>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>704</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>479</v>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>福建省少年儿童图书馆金山街道鑫龙社区分馆</t>
         </is>
       </c>
-      <c r="I6" t="n">
-        <v>0.05228704727139491</v>
+      <c r="J6" t="n">
+        <v>0.949387713739693</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>金山街道金河社区</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>福州市仓山区金山街道金山大道287号</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>6500</v>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>金洲社区卫生服务站</t>
         </is>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>887</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>286</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>金山街道金河社区</t>
         </is>
       </c>
-      <c r="I7" t="n">
-        <v>0.03637943771592936</v>
+      <c r="J7" t="n">
+        <v>0.6605496581398433</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>金山街道香江社区</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>仓山区金桔路230号水印长天25号底层08店旁香江社区</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>13620</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>中天社区卫生服务站</t>
         </is>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>163</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>569</v>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>香江社区</t>
         </is>
       </c>
-      <c r="I8" t="n">
-        <v>0.04580161226689081</v>
+      <c r="J8" t="n">
+        <v>0.8316302071898446</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="inlineStr">
         <is>
           <t>金山街道建中社区</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>福州市仓山区卢滨路639号美林湾40号楼外围商铺</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>24120</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>丽景社区卫生服务站</t>
         </is>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>577</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>718</v>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>美林湾-40栋</t>
         </is>
       </c>
-      <c r="I9" t="n">
-        <v>0.05228704727139491</v>
+      <c r="J9" t="n">
+        <v>0.949387713739693</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="inlineStr">
         <is>
           <t>金山街道新筑社区</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>福州市仓山区凤冈路569号融晟红郡小区北门二楼</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>24000</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>水都社区卫生服务站</t>
         </is>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>1065</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>816</v>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>融晟红郡-北门</t>
         </is>
       </c>
-      <c r="I10" t="n">
-        <v>0.05507449329150597</v>
+      <c r="J10" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="inlineStr">
         <is>
           <t>金山街道中天社区</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>福州市仓山区金山街道桔路三路131号</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>13563</v>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>中天社区卫生服务站</t>
         </is>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>381</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>826</v>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>中天社区居民委员会</t>
         </is>
       </c>
-      <c r="I11" t="n">
-        <v>0.04580161226689081</v>
+      <c r="J11" t="n">
+        <v>0.8316302071898446</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" t="inlineStr">
         <is>
           <t>金山街道吉龙社区</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>福州市仓山区滨洲路15号吉苑C9一层吉龙社区</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>10754</v>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>中天社区卫生服务站</t>
         </is>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>466</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>467</v>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>吉龙社区</t>
         </is>
       </c>
-      <c r="I12" t="n">
-        <v>0.04580161226689081</v>
+      <c r="J12" t="n">
+        <v>0.8316302071898446</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" t="n">
+        <v>11</v>
+      </c>
+      <c r="C13" t="inlineStr">
         <is>
           <t>金山街道潘厝社区</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>金山大道619号新榕金城湾3至4号楼连接处</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>11178</v>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>中天社区卫生服务站</t>
         </is>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>312</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>332</v>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>新榕金城湾</t>
         </is>
       </c>
-      <c r="I13" t="n">
-        <v>0.04580161226689081</v>
+      <c r="J13" t="n">
+        <v>0.8316302071898446</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" t="n">
+        <v>12</v>
+      </c>
+      <c r="C14" t="inlineStr">
         <is>
           <t>金山街道水都社区</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>仓山区闽江大道197号江南水都配套楼一层</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>12546</v>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>水都社区卫生服务站</t>
         </is>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>1742</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>578</v>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>江南水都</t>
         </is>
       </c>
-      <c r="I14" t="n">
-        <v>0.05507449329150597</v>
+      <c r="J14" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" t="n">
+        <v>13</v>
+      </c>
+      <c r="C15" t="inlineStr">
         <is>
           <t>金山街道建兴洋社区</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>福建省福州市仓山区金康路159号中庚城C区25栋一层</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>8321</v>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>丽景社区卫生服务站</t>
         </is>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>1118</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>668</v>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>中庚城-C区</t>
         </is>
       </c>
-      <c r="I15" t="n">
-        <v>0.05228704727139491</v>
+      <c r="J15" t="n">
+        <v>0.949387713739693</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" t="n">
+        <v>14</v>
+      </c>
+      <c r="C16" t="inlineStr">
         <is>
           <t>金山街道凤岗里社区</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>福建省福州市仓山区金洲南路550号金建小区一期</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
         <is>
           <t>水都社区卫生服务站</t>
         </is>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>1262</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>864</v>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>金建小区-一期</t>
         </is>
       </c>
-      <c r="I16" t="n">
-        <v>0.05507449329150597</v>
+      <c r="J16" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" t="n">
+        <v>15</v>
+      </c>
+      <c r="C17" t="inlineStr">
         <is>
           <t>金山街道百花社区</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>福建省福州市仓山区卢滨路639美林湾</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
         <is>
           <t>丽景社区卫生服务站</t>
         </is>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>647</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>625</v>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>美林湾</t>
         </is>
       </c>
-      <c r="I17" t="n">
-        <v>0.05228704727139491</v>
+      <c r="J17" t="n">
+        <v>0.949387713739693</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" t="n">
+        <v>16</v>
+      </c>
+      <c r="C18" t="inlineStr">
         <is>
           <t>金山街道横江渡社区</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>福建省福州市仓山区金山街道亭头路319号</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr">
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
         <is>
           <t>水都社区卫生服务站</t>
         </is>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>1419</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>812</v>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>TXX眼镜配镜中心(福州店)</t>
         </is>
       </c>
-      <c r="I18" t="n">
-        <v>0.05507449329150597</v>
+      <c r="J18" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" t="n">
+        <v>17</v>
+      </c>
+      <c r="C19" t="inlineStr">
         <is>
           <t>金山街道金麟社区</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>金康路150号麒麟苑16号楼</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>6218</v>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>金洲社区卫生服务站</t>
         </is>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>935</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>510</v>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>麒麟苑-16号楼</t>
         </is>
       </c>
-      <c r="I19" t="n">
-        <v>0.03637943771592936</v>
+      <c r="J19" t="n">
+        <v>0.6605496581398433</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" t="n">
+        <v>18</v>
+      </c>
+      <c r="C20" t="inlineStr">
         <is>
           <t>金山街道彼岸社区</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>福州市仓山区金山街道卢滨支路87号</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>11700</v>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>金洲社区卫生服务站</t>
         </is>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>1122</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>484</v>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>彼岸居家养老服务中心</t>
         </is>
       </c>
-      <c r="I20" t="n">
-        <v>0.03637943771592936</v>
+      <c r="J20" t="n">
+        <v>0.6605496581398433</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" t="n">
+        <v>19</v>
+      </c>
+      <c r="C21" t="inlineStr">
         <is>
           <t>金山街道金骏社区</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>福州市仓山区亭头路319号万达B1区3号楼-4号楼中间裙楼</t>
         </is>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>12069</v>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>水都社区卫生服务站</t>
         </is>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>1439</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>780</v>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>万达B1区-B3号楼</t>
         </is>
       </c>
-      <c r="I21" t="n">
-        <v>0.05507449329150597</v>
+      <c r="J21" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" t="n">
+        <v>20</v>
+      </c>
+      <c r="C22" t="inlineStr">
         <is>
           <t>金山街道丽景社区</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>福州市仓山区金山街道金山大道415号</t>
         </is>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>10790</v>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>丽景社区卫生服务站</t>
         </is>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>751</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>271</v>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="I22" t="inlineStr">
         <is>
           <t>金山街道丽景社区劳动保障工作站</t>
         </is>
       </c>
-      <c r="I22" t="n">
-        <v>0.05228704727139491</v>
+      <c r="J22" t="n">
+        <v>0.949387713739693</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
draw on the map
</commit_message>
<xml_diff>
--- a/community.xlsx
+++ b/community.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,45 +436,50 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Unnamed: 0</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>社区名称</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>地址</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>常住人口</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>发热诊室</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>标记名称</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>w</t>
         </is>
@@ -487,37 +492,40 @@
       <c r="B2" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>金山街道金洲社区</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>福州市仓山区金环路5号</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>8500</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>金洲社区卫生服务站</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>1154</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>283</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>福建省福州市仓山区金环路5号</t>
         </is>
       </c>
-      <c r="J2" t="n">
-        <v>0.6605496581398433</v>
+      <c r="K2" t="n">
+        <v>0.628755332307389</v>
       </c>
     </row>
     <row r="3">
@@ -527,37 +535,40 @@
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>金山街道幸福社区</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>仓山区浦上大道418号泰禾红峪A14号楼一层</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>7850</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>丽景社区卫生服务站</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>801</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>945</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>福建省福州市仓山区葛屿路</t>
         </is>
       </c>
-      <c r="J3" t="n">
-        <v>0.949387713739693</v>
+      <c r="K3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -567,37 +578,40 @@
       <c r="B4" t="n">
         <v>2</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>金山街道六江道社区</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>福州市仓山区金桔路826号68栋旁</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>6900</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>中天社区卫生服务站</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>432</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>980</v>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>福建省福州市仓山区金桔路</t>
         </is>
       </c>
-      <c r="J4" t="n">
-        <v>0.8316302071898446</v>
+      <c r="K4" t="n">
+        <v>0.7958665147463901</v>
       </c>
     </row>
     <row r="5">
@@ -607,37 +621,40 @@
       <c r="B5" t="n">
         <v>3</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>金山街道金环社区</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>福州市仓山区金山街道金榕南路10号榕城广场8号楼一层</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>10832</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>金洲社区卫生服务站</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>1303</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>256</v>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>福建省福州市仓山区友兰路</t>
         </is>
       </c>
-      <c r="J5" t="n">
-        <v>0.6605496581398433</v>
+      <c r="K5" t="n">
+        <v>0.628755332307389</v>
       </c>
     </row>
     <row r="6">
@@ -647,37 +664,40 @@
       <c r="B6" t="n">
         <v>4</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>金山街道鑫龙社区</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>福州市仓山区石边支路1号</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>9000</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>丽景社区卫生服务站</t>
         </is>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>704</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>479</v>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>福建省少年儿童图书馆金山街道鑫龙社区分馆</t>
         </is>
       </c>
-      <c r="J6" t="n">
-        <v>0.949387713739693</v>
+      <c r="K6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -687,37 +707,40 @@
       <c r="B7" t="n">
         <v>5</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>金山街道金河社区</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>福州市仓山区金山街道金山大道287号</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>6500</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>金洲社区卫生服务站</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>887</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>286</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>金山街道金河社区</t>
         </is>
       </c>
-      <c r="J7" t="n">
-        <v>0.6605496581398433</v>
+      <c r="K7" t="n">
+        <v>0.628755332307389</v>
       </c>
     </row>
     <row r="8">
@@ -727,37 +750,40 @@
       <c r="B8" t="n">
         <v>6</v>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>金山街道香江社区</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>仓山区金桔路230号水印长天25号底层08店旁香江社区</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>13620</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>中天社区卫生服务站</t>
         </is>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>163</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>569</v>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>香江社区</t>
         </is>
       </c>
-      <c r="J8" t="n">
-        <v>0.8316302071898446</v>
+      <c r="K8" t="n">
+        <v>0.7958665147463901</v>
       </c>
     </row>
     <row r="9">
@@ -767,37 +793,40 @@
       <c r="B9" t="n">
         <v>7</v>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>金山街道建中社区</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>福州市仓山区卢滨路639号美林湾40号楼外围商铺</t>
         </is>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>24120</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>丽景社区卫生服务站</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>577</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>718</v>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>美林湾-40栋</t>
         </is>
       </c>
-      <c r="J9" t="n">
-        <v>0.949387713739693</v>
+      <c r="K9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -807,37 +836,40 @@
       <c r="B10" t="n">
         <v>8</v>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>金山街道新筑社区</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>福州市仓山区凤冈路569号融晟红郡小区北门二楼</t>
         </is>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>24000</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>水都社区卫生服务站</t>
         </is>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>1065</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>816</v>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>融晟红郡-北门</t>
         </is>
       </c>
-      <c r="J10" t="n">
-        <v>1</v>
+      <c r="K10" t="n">
+        <v>0.9650740266112243</v>
       </c>
     </row>
     <row r="11">
@@ -847,37 +879,40 @@
       <c r="B11" t="n">
         <v>9</v>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" t="inlineStr">
         <is>
           <t>金山街道中天社区</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>福州市仓山区金山街道桔路三路131号</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>13563</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>中天社区卫生服务站</t>
         </is>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>381</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>826</v>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>中天社区居民委员会</t>
         </is>
       </c>
-      <c r="J11" t="n">
-        <v>0.8316302071898446</v>
+      <c r="K11" t="n">
+        <v>0.7958665147463901</v>
       </c>
     </row>
     <row r="12">
@@ -887,37 +922,40 @@
       <c r="B12" t="n">
         <v>10</v>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" t="n">
+        <v>10</v>
+      </c>
+      <c r="D12" t="inlineStr">
         <is>
           <t>金山街道吉龙社区</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>福州市仓山区滨洲路15号吉苑C9一层吉龙社区</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>10754</v>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>中天社区卫生服务站</t>
         </is>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>466</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>467</v>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>吉龙社区</t>
         </is>
       </c>
-      <c r="J12" t="n">
-        <v>0.8316302071898446</v>
+      <c r="K12" t="n">
+        <v>0.7958665147463901</v>
       </c>
     </row>
     <row r="13">
@@ -927,37 +965,40 @@
       <c r="B13" t="n">
         <v>11</v>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" t="n">
+        <v>11</v>
+      </c>
+      <c r="D13" t="inlineStr">
         <is>
           <t>金山街道潘厝社区</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>金山大道619号新榕金城湾3至4号楼连接处</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>11178</v>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>中天社区卫生服务站</t>
         </is>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>312</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>332</v>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>新榕金城湾</t>
         </is>
       </c>
-      <c r="J13" t="n">
-        <v>0.8316302071898446</v>
+      <c r="K13" t="n">
+        <v>0.7958665147463901</v>
       </c>
     </row>
     <row r="14">
@@ -967,37 +1008,40 @@
       <c r="B14" t="n">
         <v>12</v>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" t="n">
+        <v>12</v>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>金山街道水都社区</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>仓山区闽江大道197号江南水都配套楼一层</t>
         </is>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>12546</v>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>水都社区卫生服务站</t>
         </is>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>1742</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>578</v>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>江南水都</t>
         </is>
       </c>
-      <c r="J14" t="n">
-        <v>1</v>
+      <c r="K14" t="n">
+        <v>0.9650740266112243</v>
       </c>
     </row>
     <row r="15">
@@ -1007,37 +1051,40 @@
       <c r="B15" t="n">
         <v>13</v>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" t="n">
+        <v>13</v>
+      </c>
+      <c r="D15" t="inlineStr">
         <is>
           <t>金山街道建兴洋社区</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>福建省福州市仓山区金康路159号中庚城C区25栋一层</t>
         </is>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>8321</v>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>丽景社区卫生服务站</t>
         </is>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>1118</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>668</v>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>中庚城-C区</t>
         </is>
       </c>
-      <c r="J15" t="n">
-        <v>0.949387713739693</v>
+      <c r="K15" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -1047,35 +1094,38 @@
       <c r="B16" t="n">
         <v>14</v>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" t="n">
+        <v>14</v>
+      </c>
+      <c r="D16" t="inlineStr">
         <is>
           <t>金山街道凤岗里社区</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>福建省福州市仓山区金洲南路550号金建小区一期</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
         <is>
           <t>水都社区卫生服务站</t>
         </is>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>1262</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>864</v>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>金建小区-一期</t>
         </is>
       </c>
-      <c r="J16" t="n">
-        <v>1</v>
+      <c r="K16" t="n">
+        <v>0.9650740266112243</v>
       </c>
     </row>
     <row r="17">
@@ -1085,35 +1135,38 @@
       <c r="B17" t="n">
         <v>15</v>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" t="n">
+        <v>15</v>
+      </c>
+      <c r="D17" t="inlineStr">
         <is>
           <t>金山街道百花社区</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>福建省福州市仓山区卢滨路639美林湾</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr">
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
         <is>
           <t>丽景社区卫生服务站</t>
         </is>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>647</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>625</v>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>美林湾</t>
         </is>
       </c>
-      <c r="J17" t="n">
-        <v>0.949387713739693</v>
+      <c r="K17" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1123,35 +1176,38 @@
       <c r="B18" t="n">
         <v>16</v>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" t="n">
+        <v>16</v>
+      </c>
+      <c r="D18" t="inlineStr">
         <is>
           <t>金山街道横江渡社区</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>福建省福州市仓山区金山街道亭头路319号</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr">
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
         <is>
           <t>水都社区卫生服务站</t>
         </is>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>1419</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>812</v>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>TXX眼镜配镜中心(福州店)</t>
         </is>
       </c>
-      <c r="J18" t="n">
-        <v>1</v>
+      <c r="K18" t="n">
+        <v>0.9650740266112243</v>
       </c>
     </row>
     <row r="19">
@@ -1161,37 +1217,40 @@
       <c r="B19" t="n">
         <v>17</v>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" t="n">
+        <v>17</v>
+      </c>
+      <c r="D19" t="inlineStr">
         <is>
           <t>金山街道金麟社区</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>金康路150号麒麟苑16号楼</t>
         </is>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>6218</v>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>金洲社区卫生服务站</t>
         </is>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>935</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>510</v>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>麒麟苑-16号楼</t>
         </is>
       </c>
-      <c r="J19" t="n">
-        <v>0.6605496581398433</v>
+      <c r="K19" t="n">
+        <v>0.628755332307389</v>
       </c>
     </row>
     <row r="20">
@@ -1201,37 +1260,40 @@
       <c r="B20" t="n">
         <v>18</v>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" t="n">
+        <v>18</v>
+      </c>
+      <c r="D20" t="inlineStr">
         <is>
           <t>金山街道彼岸社区</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>福州市仓山区金山街道卢滨支路87号</t>
         </is>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>11700</v>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>金洲社区卫生服务站</t>
         </is>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>1122</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>484</v>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>彼岸居家养老服务中心</t>
         </is>
       </c>
-      <c r="J20" t="n">
-        <v>0.6605496581398433</v>
+      <c r="K20" t="n">
+        <v>0.628755332307389</v>
       </c>
     </row>
     <row r="21">
@@ -1241,37 +1303,40 @@
       <c r="B21" t="n">
         <v>19</v>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" t="n">
+        <v>19</v>
+      </c>
+      <c r="D21" t="inlineStr">
         <is>
           <t>金山街道金骏社区</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>福州市仓山区亭头路319号万达B1区3号楼-4号楼中间裙楼</t>
         </is>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>12069</v>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>水都社区卫生服务站</t>
         </is>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>1439</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>780</v>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>万达B1区-B3号楼</t>
         </is>
       </c>
-      <c r="J21" t="n">
-        <v>1</v>
+      <c r="K21" t="n">
+        <v>0.9650740266112243</v>
       </c>
     </row>
     <row r="22">
@@ -1281,37 +1346,40 @@
       <c r="B22" t="n">
         <v>20</v>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" t="n">
+        <v>20</v>
+      </c>
+      <c r="D22" t="inlineStr">
         <is>
           <t>金山街道丽景社区</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>福州市仓山区金山街道金山大道415号</t>
         </is>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>10790</v>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>丽景社区卫生服务站</t>
         </is>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>751</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>271</v>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="J22" t="inlineStr">
         <is>
           <t>金山街道丽景社区劳动保障工作站</t>
         </is>
       </c>
-      <c r="J22" t="n">
-        <v>0.949387713739693</v>
+      <c r="K22" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>